<commit_message>
done all todos except one
</commit_message>
<xml_diff>
--- a/assets/uploads/3f000935-97eb-4868-8d49-5c38a633e327.xlsx
+++ b/assets/uploads/3f000935-97eb-4868-8d49-5c38a633e327.xlsx
@@ -53,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -75,12 +75,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,7 +119,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -134,12 +128,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -162,7 +152,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -195,18 +185,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>